<commit_message>
Some change in binary file
</commit_message>
<xml_diff>
--- a/Materiaali.xlsx
+++ b/Materiaali.xlsx
@@ -4811,8 +4811,8 @@
   <dimension ref="A1:AL130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>